<commit_message>
Change the value in excel sheet
</commit_message>
<xml_diff>
--- a/src/test/java/com/finacus/TestCase/travalab.xlsx
+++ b/src/test/java/com/finacus/TestCase/travalab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FIN_MobiConnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340AD00A-4A5A-4D73-BBF3-19340C999520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB09CE8-FB6F-46A2-9E2F-1959DDC0096C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="2640" windowWidth="15375" windowHeight="7875" xr2:uid="{CB2EF90B-94E9-453E-BEB2-6FC469B71AB3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>password</t>
   </si>
@@ -409,7 +409,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,16 +430,21 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>